<commit_message>
UMLs added working on Tiles
project still compiles!
</commit_message>
<xml_diff>
--- a/Resources/Boards/DockingBay.xlsx
+++ b/Resources/Boards/DockingBay.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,12 +16,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t xml:space="preserve">BaseSpriteSheet </t>
   </si>
   <si>
     <t xml:space="preserve">floor </t>
+  </si>
+  <si>
+    <t>conv 270 1</t>
+  </si>
+  <si>
+    <t>convr 270 1</t>
+  </si>
+  <si>
+    <t>convl 180 1</t>
+  </si>
+  <si>
+    <t>conv 90 1</t>
+  </si>
+  <si>
+    <t>convr 180 1</t>
+  </si>
+  <si>
+    <t>convl 90 1</t>
+  </si>
+  <si>
+    <t>floor wall 0</t>
+  </si>
+  <si>
+    <t>floor wall 0 90</t>
+  </si>
+  <si>
+    <t>floor wall 90</t>
+  </si>
+  <si>
+    <t>floor wall 270</t>
+  </si>
+  <si>
+    <t>floor wall 0 270</t>
+  </si>
+  <si>
+    <t>floor start 8</t>
+  </si>
+  <si>
+    <t>floor wall 90 start 6</t>
+  </si>
+  <si>
+    <t>floor start 4</t>
+  </si>
+  <si>
+    <t>floor wall 270 start 2</t>
+  </si>
+  <si>
+    <t>floor start 1</t>
+  </si>
+  <si>
+    <t>floor start 3</t>
+  </si>
+  <si>
+    <t>floor wall 270 start 5</t>
+  </si>
+  <si>
+    <t>floor start 7</t>
   </si>
 </sst>
 </file>
@@ -37,12 +94,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -57,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,34 +417,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="30.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" customHeight="1">
+    <row r="1" spans="1:12" ht="53.25" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30.75" customHeight="1">
+    <row r="2" spans="1:12" ht="53.25" customHeight="1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -389,30 +453,30 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30.75" customHeight="1">
+    <row r="3" spans="1:12" ht="53.25" customHeight="1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -433,27 +497,27 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="L3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30.75" customHeight="1">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
+    <row r="4" spans="1:12" ht="53.25" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -462,54 +526,54 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30.75" customHeight="1">
+    <row r="5" spans="1:12" ht="53.25" customHeight="1">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="K5" t="s">
         <v>1</v>
@@ -518,6 +582,9 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:12" ht="53.25" customHeight="1"/>
+    <row r="7" spans="1:12" ht="53.25" customHeight="1"/>
+    <row r="8" spans="1:12" ht="53.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
mostly boards orientation and tiles parcing and logic
new maps csv
new boards orientation logic (old code commented)
a bunch of clean up of silly tiles logic test stuff
new tiles logic with better testing
</commit_message>
<xml_diff>
--- a/Resources/Boards/DockingBay.xlsx
+++ b/Resources/Boards/DockingBay.xlsx
@@ -27,21 +27,9 @@
     <t>conv 270 1</t>
   </si>
   <si>
-    <t>convr 270 1</t>
-  </si>
-  <si>
-    <t>convl 180 1</t>
-  </si>
-  <si>
     <t>conv 90 1</t>
   </si>
   <si>
-    <t>convr 180 1</t>
-  </si>
-  <si>
-    <t>convl 90 1</t>
-  </si>
-  <si>
     <t>floor wall 0</t>
   </si>
   <si>
@@ -79,6 +67,18 @@
   </si>
   <si>
     <t>floor start 7</t>
+  </si>
+  <si>
+    <t>convbl 180 1</t>
+  </si>
+  <si>
+    <t>convbr 270 1</t>
+  </si>
+  <si>
+    <t>convbr 180 1</t>
+  </si>
+  <si>
+    <t>convbl 90 1</t>
   </si>
 </sst>
 </file>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="30.75" customHeight="1"/>
@@ -432,20 +432,20 @@
     </row>
     <row r="2" spans="1:12" ht="53.25" customHeight="1">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
         <v>1</v>
       </c>
@@ -453,19 +453,19 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
         <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="53.25" customHeight="1">
@@ -473,10 +473,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -497,10 +497,10 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
         <v>10</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
       </c>
       <c r="L3" t="s">
         <v>1</v>
@@ -508,16 +508,16 @@
     </row>
     <row r="4" spans="1:12" ht="53.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -526,16 +526,16 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>2</v>
@@ -552,19 +552,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>2</v>
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="K5" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
sprite sheet, tile and tile feature
chop shop and docking bay prinet!

made small adjustment to robot.h as it uses tilefeature constructor
(which i changed)
</commit_message>
<xml_diff>
--- a/Resources/Boards/DockingBay.xlsx
+++ b/Resources/Boards/DockingBay.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -27,42 +27,18 @@
     <t>conv 90 1</t>
   </si>
   <si>
-    <t>floor wall 0</t>
-  </si>
-  <si>
-    <t>floor wall 0 90</t>
-  </si>
-  <si>
-    <t>floor wall 90</t>
-  </si>
-  <si>
-    <t>floor wall 270</t>
-  </si>
-  <si>
-    <t>floor wall 0 270</t>
-  </si>
-  <si>
     <t>floor start 8</t>
   </si>
   <si>
-    <t>floor wall 90 start 6</t>
-  </si>
-  <si>
     <t>floor start 4</t>
   </si>
   <si>
-    <t>floor wall 270 start 2</t>
-  </si>
-  <si>
     <t>floor start 1</t>
   </si>
   <si>
     <t>floor start 3</t>
   </si>
   <si>
-    <t>floor wall 270 start 5</t>
-  </si>
-  <si>
     <t>floor start 7</t>
   </si>
   <si>
@@ -79,6 +55,30 @@
   </si>
   <si>
     <t>boardSpriteSheet.png</t>
+  </si>
+  <si>
+    <t>floor wall 0 0</t>
+  </si>
+  <si>
+    <t>floor wall 270 0</t>
+  </si>
+  <si>
+    <t>floor wall 0 0 wall 90 0</t>
+  </si>
+  <si>
+    <t>floor wall 0 0 wall 270 0</t>
+  </si>
+  <si>
+    <t>floor wall 270 0 start 5</t>
+  </si>
+  <si>
+    <t>floor wall 270 0 start 2</t>
+  </si>
+  <si>
+    <t>floor wall 90 0</t>
+  </si>
+  <si>
+    <t>floor wall 90 0 start 6</t>
   </si>
 </sst>
 </file>
@@ -419,51 +419,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="30.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="30.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:12" ht="53.25" customHeight="1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="53.25" customHeight="1">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="53.25" customHeight="1">
@@ -471,11 +473,11 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -495,10 +497,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="L3" t="s">
         <v>0</v>
@@ -512,28 +514,28 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>1</v>
@@ -550,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -559,10 +561,10 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>1</v>
@@ -571,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K5" t="s">
         <v>0</v>
@@ -594,7 +596,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -606,7 +608,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>